<commit_message>
minor changes to the scripts
</commit_message>
<xml_diff>
--- a/subject_info.xlsx
+++ b/subject_info.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,10 +456,15 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>StimOrder</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Sex</t>
         </is>
@@ -485,9 +490,12 @@
         </is>
       </c>
       <c r="E2" t="n">
+        <v>321</v>
+      </c>
+      <c r="F2" t="n">
         <v>30.83</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -513,9 +521,12 @@
         </is>
       </c>
       <c r="E3" t="n">
+        <v>312</v>
+      </c>
+      <c r="F3" t="n">
         <v>32.01</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -541,9 +552,12 @@
         </is>
       </c>
       <c r="E4" t="n">
+        <v>132</v>
+      </c>
+      <c r="F4" t="n">
         <v>26.19</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -569,9 +583,12 @@
         </is>
       </c>
       <c r="E5" t="n">
+        <v>321</v>
+      </c>
+      <c r="F5" t="n">
         <v>22.32</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -597,9 +614,12 @@
         </is>
       </c>
       <c r="E6" t="n">
+        <v>321</v>
+      </c>
+      <c r="F6" t="n">
         <v>23.62</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -625,9 +645,12 @@
         </is>
       </c>
       <c r="E7" t="n">
+        <v>123</v>
+      </c>
+      <c r="F7" t="n">
         <v>20.89</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -653,9 +676,12 @@
         </is>
       </c>
       <c r="E8" t="n">
+        <v>231</v>
+      </c>
+      <c r="F8" t="n">
         <v>33</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -681,9 +707,12 @@
         </is>
       </c>
       <c r="E9" t="n">
+        <v>231</v>
+      </c>
+      <c r="F9" t="n">
         <v>26.62</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -709,9 +738,12 @@
         </is>
       </c>
       <c r="E10" t="n">
+        <v>231</v>
+      </c>
+      <c r="F10" t="n">
         <v>22.37</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -737,9 +769,12 @@
         </is>
       </c>
       <c r="E11" t="n">
+        <v>213</v>
+      </c>
+      <c r="F11" t="n">
         <v>26.39</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -765,9 +800,12 @@
         </is>
       </c>
       <c r="E12" t="n">
+        <v>321</v>
+      </c>
+      <c r="F12" t="n">
         <v>21.42</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -793,9 +831,12 @@
         </is>
       </c>
       <c r="E13" t="n">
+        <v>213</v>
+      </c>
+      <c r="F13" t="n">
         <v>27.75</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -821,9 +862,12 @@
         </is>
       </c>
       <c r="E14" t="n">
+        <v>213</v>
+      </c>
+      <c r="F14" t="n">
         <v>31.01</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -849,9 +893,12 @@
         </is>
       </c>
       <c r="E15" t="n">
+        <v>132</v>
+      </c>
+      <c r="F15" t="n">
         <v>28.14</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -877,9 +924,12 @@
         </is>
       </c>
       <c r="E16" t="n">
+        <v>123</v>
+      </c>
+      <c r="F16" t="n">
         <v>22.35</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -905,9 +955,12 @@
         </is>
       </c>
       <c r="E17" t="n">
+        <v>123</v>
+      </c>
+      <c r="F17" t="n">
         <v>29.88</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -933,9 +986,12 @@
         </is>
       </c>
       <c r="E18" t="n">
+        <v>321</v>
+      </c>
+      <c r="F18" t="n">
         <v>19.98</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -961,9 +1017,12 @@
         </is>
       </c>
       <c r="E19" t="n">
+        <v>213</v>
+      </c>
+      <c r="F19" t="n">
         <v>22.21</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -989,9 +1048,12 @@
         </is>
       </c>
       <c r="E20" t="n">
+        <v>123</v>
+      </c>
+      <c r="F20" t="n">
         <v>23.1</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1017,9 +1079,12 @@
         </is>
       </c>
       <c r="E21" t="n">
+        <v>123</v>
+      </c>
+      <c r="F21" t="n">
         <v>25.28</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1045,9 +1110,12 @@
         </is>
       </c>
       <c r="E22" t="n">
+        <v>312</v>
+      </c>
+      <c r="F22" t="n">
         <v>28.95</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1073,9 +1141,12 @@
         </is>
       </c>
       <c r="E23" t="n">
+        <v>213</v>
+      </c>
+      <c r="F23" t="n">
         <v>25.96</v>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1101,9 +1172,12 @@
         </is>
       </c>
       <c r="E24" t="n">
+        <v>123</v>
+      </c>
+      <c r="F24" t="n">
         <v>25.45</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1129,9 +1203,12 @@
         </is>
       </c>
       <c r="E25" t="n">
+        <v>321</v>
+      </c>
+      <c r="F25" t="n">
         <v>24.79</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1157,9 +1234,12 @@
         </is>
       </c>
       <c r="E26" t="n">
+        <v>231</v>
+      </c>
+      <c r="F26" t="n">
         <v>19.96</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1185,9 +1265,12 @@
         </is>
       </c>
       <c r="E27" t="n">
+        <v>312</v>
+      </c>
+      <c r="F27" t="n">
         <v>20.21</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1213,9 +1296,12 @@
         </is>
       </c>
       <c r="E28" t="n">
+        <v>321</v>
+      </c>
+      <c r="F28" t="n">
         <v>39.62</v>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1241,9 +1327,12 @@
         </is>
       </c>
       <c r="E29" t="n">
+        <v>213</v>
+      </c>
+      <c r="F29" t="n">
         <v>31.9</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1269,9 +1358,12 @@
         </is>
       </c>
       <c r="E30" t="n">
+        <v>132</v>
+      </c>
+      <c r="F30" t="n">
         <v>21.37</v>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1297,9 +1389,12 @@
         </is>
       </c>
       <c r="E31" t="n">
+        <v>312</v>
+      </c>
+      <c r="F31" t="n">
         <v>19.7</v>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1325,9 +1420,12 @@
         </is>
       </c>
       <c r="E32" t="n">
+        <v>132</v>
+      </c>
+      <c r="F32" t="n">
         <v>22.98</v>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1353,9 +1451,12 @@
         </is>
       </c>
       <c r="E33" t="n">
+        <v>123</v>
+      </c>
+      <c r="F33" t="n">
         <v>26.14</v>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1381,9 +1482,12 @@
         </is>
       </c>
       <c r="E34" t="n">
+        <v>213</v>
+      </c>
+      <c r="F34" t="n">
         <v>26.62</v>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1409,9 +1513,12 @@
         </is>
       </c>
       <c r="E35" t="n">
+        <v>132</v>
+      </c>
+      <c r="F35" t="n">
         <v>23.29</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1437,9 +1544,12 @@
         </is>
       </c>
       <c r="E36" t="n">
+        <v>312</v>
+      </c>
+      <c r="F36" t="n">
         <v>25.01</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1465,9 +1575,12 @@
         </is>
       </c>
       <c r="E37" t="n">
+        <v>123</v>
+      </c>
+      <c r="F37" t="n">
         <v>25.76</v>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1493,9 +1606,12 @@
         </is>
       </c>
       <c r="E38" t="n">
+        <v>312</v>
+      </c>
+      <c r="F38" t="n">
         <v>25.29</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1521,9 +1637,12 @@
         </is>
       </c>
       <c r="E39" t="n">
+        <v>213</v>
+      </c>
+      <c r="F39" t="n">
         <v>25.24</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1549,9 +1668,12 @@
         </is>
       </c>
       <c r="E40" t="n">
+        <v>132</v>
+      </c>
+      <c r="F40" t="n">
         <v>26.28</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1577,9 +1699,12 @@
         </is>
       </c>
       <c r="E41" t="n">
+        <v>231</v>
+      </c>
+      <c r="F41" t="n">
         <v>26.13</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1605,9 +1730,12 @@
         </is>
       </c>
       <c r="E42" t="n">
+        <v>231</v>
+      </c>
+      <c r="F42" t="n">
         <v>27.05</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="G42" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1633,9 +1761,12 @@
         </is>
       </c>
       <c r="E43" t="n">
+        <v>231</v>
+      </c>
+      <c r="F43" t="n">
         <v>23.53</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1661,9 +1792,12 @@
         </is>
       </c>
       <c r="E44" t="n">
+        <v>312</v>
+      </c>
+      <c r="F44" t="n">
         <v>23.53</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1689,9 +1823,12 @@
         </is>
       </c>
       <c r="E45" t="n">
+        <v>312</v>
+      </c>
+      <c r="F45" t="n">
         <v>20.19</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1717,9 +1854,12 @@
         </is>
       </c>
       <c r="E46" t="n">
+        <v>132</v>
+      </c>
+      <c r="F46" t="n">
         <v>20.03</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1745,9 +1885,12 @@
         </is>
       </c>
       <c r="E47" t="n">
+        <v>123</v>
+      </c>
+      <c r="F47" t="n">
         <v>18.1</v>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -1773,9 +1916,12 @@
         </is>
       </c>
       <c r="E48" t="n">
+        <v>321</v>
+      </c>
+      <c r="F48" t="n">
         <v>24.51</v>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="G48" t="inlineStr">
         <is>
           <t>F</t>
         </is>
@@ -1801,9 +1947,12 @@
         </is>
       </c>
       <c r="E49" t="n">
+        <v>231</v>
+      </c>
+      <c r="F49" t="n">
         <v>25.24</v>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="G49" t="inlineStr">
         <is>
           <t>F</t>
         </is>

</xml_diff>